<commit_message>
Updated code for Explore project
</commit_message>
<xml_diff>
--- a/erb/app/src/main/resources/staticData/directoryIDs.xlsx
+++ b/erb/app/src/main/resources/staticData/directoryIDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\Equitable-Resilience-Builder-GUI\erb_supporting_docs\Code_Resources\ERB\Static_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\Equitable-Resilience-Builder-GUI\erb\app\src\main\resources\staticData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0BEAE0-8DCA-4449-A08A-9DD5DAE2AC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026F3A4C-DBCA-4D7D-9FAD-84679172BA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46245" yWindow="450" windowWidth="14700" windowHeight="15075" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="14580" yWindow="180" windowWidth="13890" windowHeight="11295" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -788,7 +788,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -891,11 +891,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -939,6 +952,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1269,9 +1283,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
   <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C195" sqref="C195"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C196" sqref="C196:C199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3547,7 +3561,7 @@
       <c r="B160" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="C160" s="3" t="s">
         <v>176</v>
       </c>
       <c r="D160" s="2" t="s">
@@ -3561,7 +3575,7 @@
       <c r="B161" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C161" s="3" t="s">
         <v>177</v>
       </c>
       <c r="D161" s="2" t="s">
@@ -3575,7 +3589,7 @@
       <c r="B162" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="3" t="s">
         <v>178</v>
       </c>
       <c r="D162" s="2" t="s">
@@ -3589,7 +3603,7 @@
       <c r="B163" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C163" s="3" t="s">
         <v>179</v>
       </c>
       <c r="D163" s="2" t="s">
@@ -3603,7 +3617,7 @@
       <c r="B164" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C164" s="3" t="s">
         <v>180</v>
       </c>
       <c r="D164" s="2" t="s">
@@ -3617,7 +3631,7 @@
       <c r="B165" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C165" s="2" t="s">
+      <c r="C165" s="3" t="s">
         <v>181</v>
       </c>
       <c r="D165" s="2" t="s">
@@ -3631,7 +3645,7 @@
       <c r="B166" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C166" s="2" t="s">
+      <c r="C166" s="3" t="s">
         <v>182</v>
       </c>
       <c r="D166" s="2" t="s">
@@ -3645,7 +3659,7 @@
       <c r="B167" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C167" s="3" t="s">
         <v>183</v>
       </c>
       <c r="D167" s="2" t="s">
@@ -3659,7 +3673,7 @@
       <c r="B168" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="C168" s="3" t="s">
         <v>184</v>
       </c>
       <c r="D168" s="2" t="s">
@@ -3673,7 +3687,7 @@
       <c r="B169" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C169" s="3" t="s">
         <v>185</v>
       </c>
       <c r="D169" s="2" t="s">
@@ -3687,7 +3701,7 @@
       <c r="B170" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="C170" s="3" t="s">
         <v>186</v>
       </c>
       <c r="D170" s="2" t="s">
@@ -3701,7 +3715,7 @@
       <c r="B171" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="3" t="s">
         <v>187</v>
       </c>
       <c r="D171" s="2" t="s">
@@ -3715,7 +3729,7 @@
       <c r="B172" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C172" s="3" t="s">
         <v>188</v>
       </c>
       <c r="D172" s="2" t="s">
@@ -3729,7 +3743,7 @@
       <c r="B173" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C173" s="3" t="s">
         <v>189</v>
       </c>
       <c r="D173" s="2" t="s">
@@ -3743,7 +3757,7 @@
       <c r="B174" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C174" s="3" t="s">
         <v>190</v>
       </c>
       <c r="D174" s="2" t="s">
@@ -3757,7 +3771,7 @@
       <c r="B175" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C175" s="3" t="s">
         <v>191</v>
       </c>
       <c r="D175" s="2" t="s">
@@ -3771,7 +3785,7 @@
       <c r="B176" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C176" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D176" s="2" t="s">
@@ -3785,7 +3799,7 @@
       <c r="B177" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C177" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D177" s="2" t="s">
@@ -3799,7 +3813,7 @@
       <c r="B178" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="C178" s="3" t="s">
         <v>194</v>
       </c>
       <c r="D178" s="2" t="s">
@@ -3813,7 +3827,7 @@
       <c r="B179" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C179" s="2" t="s">
+      <c r="C179" s="3" t="s">
         <v>195</v>
       </c>
       <c r="D179" s="2" t="s">
@@ -3827,7 +3841,7 @@
       <c r="B180" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C180" s="2" t="s">
+      <c r="C180" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D180" s="2" t="s">
@@ -3841,7 +3855,7 @@
       <c r="B181" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C181" s="3" t="s">
         <v>197</v>
       </c>
       <c r="D181" s="2" t="s">
@@ -3855,7 +3869,7 @@
       <c r="B182" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C182" s="3" t="s">
         <v>198</v>
       </c>
       <c r="D182" s="2" t="s">
@@ -3869,7 +3883,7 @@
       <c r="B183" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C183" s="2" t="s">
+      <c r="C183" s="3" t="s">
         <v>199</v>
       </c>
       <c r="D183" s="2" t="s">
@@ -3883,7 +3897,7 @@
       <c r="B184" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C184" s="2" t="s">
+      <c r="C184" s="35" t="s">
         <v>200</v>
       </c>
       <c r="D184" s="2" t="s">
@@ -3897,7 +3911,7 @@
       <c r="B185" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C185" s="2" t="s">
+      <c r="C185" s="3" t="s">
         <v>201</v>
       </c>
       <c r="D185" s="2" t="s">
@@ -3911,7 +3925,7 @@
       <c r="B186" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C186" s="2" t="s">
+      <c r="C186" s="3" t="s">
         <v>202</v>
       </c>
       <c r="D186" s="2" t="s">
@@ -3925,7 +3939,7 @@
       <c r="B187" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C187" s="2" t="s">
+      <c r="C187" s="3" t="s">
         <v>203</v>
       </c>
       <c r="D187" s="2" t="s">
@@ -3939,7 +3953,7 @@
       <c r="B188" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C188" s="2" t="s">
+      <c r="C188" s="3" t="s">
         <v>204</v>
       </c>
       <c r="D188" s="2" t="s">
@@ -3953,7 +3967,7 @@
       <c r="B189" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="C189" s="3" t="s">
         <v>205</v>
       </c>
       <c r="D189" s="2" t="s">
@@ -3967,7 +3981,7 @@
       <c r="B190" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C190" s="3" t="s">
         <v>206</v>
       </c>
       <c r="D190" s="2" t="s">
@@ -3981,7 +3995,7 @@
       <c r="B191" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="C191" s="3" t="s">
         <v>207</v>
       </c>
       <c r="D191" s="2" t="s">
@@ -3995,7 +4009,7 @@
       <c r="B192" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C192" s="2" t="s">
+      <c r="C192" s="3" t="s">
         <v>208</v>
       </c>
       <c r="D192" s="2" t="s">
@@ -4009,7 +4023,7 @@
       <c r="B193" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="C193" s="3" t="s">
         <v>209</v>
       </c>
       <c r="D193" s="2" t="s">
@@ -4023,7 +4037,7 @@
       <c r="B194" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="C194" s="3" t="s">
         <v>210</v>
       </c>
       <c r="D194" s="2" t="s">
@@ -4037,7 +4051,7 @@
       <c r="B195" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="C195" s="3" t="s">
         <v>211</v>
       </c>
       <c r="D195" s="2" t="s">
@@ -4051,7 +4065,7 @@
       <c r="B196" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="C196" s="3" t="s">
         <v>212</v>
       </c>
       <c r="D196" s="2" t="s">
@@ -4065,7 +4079,7 @@
       <c r="B197" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C197" s="2" t="s">
+      <c r="C197" s="3" t="s">
         <v>213</v>
       </c>
       <c r="D197" s="2" t="s">
@@ -4079,7 +4093,7 @@
       <c r="B198" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C198" s="2" t="s">
+      <c r="C198" s="3" t="s">
         <v>214</v>
       </c>
       <c r="D198" s="2" t="s">
@@ -4093,7 +4107,7 @@
       <c r="B199" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C199" s="2" t="s">
+      <c r="C199" s="3" t="s">
         <v>215</v>
       </c>
       <c r="D199" s="2" t="s">
@@ -4107,7 +4121,7 @@
       <c r="B200" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C200" s="2" t="s">
+      <c r="C200" s="3" t="s">
         <v>216</v>
       </c>
       <c r="D200" s="2" t="s">
@@ -4121,7 +4135,7 @@
       <c r="B201" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="C201" s="3" t="s">
         <v>217</v>
       </c>
       <c r="D201" s="2" t="s">
@@ -4135,7 +4149,7 @@
       <c r="B202" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="C202" s="2" t="s">
+      <c r="C202" s="3" t="s">
         <v>218</v>
       </c>
       <c r="D202" s="2" t="s">

</xml_diff>

<commit_message>
Updates to indicator center location, map out ERB dashboard, address bugs
</commit_message>
<xml_diff>
--- a/erb/app/src/main/resources/staticData/directoryIDs.xlsx
+++ b/erb/app/src/main/resources/staticData/directoryIDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awilke06\Documents\Eclipse_Repos\MetroCERI\Equitable-Resilience-Builder-GUI\erb\app\src\main\resources\staticData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdale\erb\desktop\Equitable-Resilience-Builder-GUI\erb\app\src\main\resources\staticData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026F3A4C-DBCA-4D7D-9FAD-84679172BA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E475E9C8-C492-4FB3-8CB7-D987A5A0F0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="180" windowWidth="13890" windowHeight="11295" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3019C20B-FC5C-4DA4-8E55-4106A73F2974}"/>
   </bookViews>
   <sheets>
     <sheet name="New_Mapping" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="218">
   <si>
     <t>ID</t>
   </si>
@@ -433,9 +433,6 @@
   </si>
   <si>
     <t>Plan Workshop 2</t>
-  </si>
-  <si>
-    <t>Sort Indicator Cards</t>
   </si>
   <si>
     <t>Assess: Reflection/Next Steps</t>
@@ -985,9 +982,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1025,7 +1022,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1131,7 +1128,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1273,7 +1270,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1281,11 +1278,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD8D25E-7481-479A-B804-CA294EBD659C}">
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C196" sqref="C196:C199"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1305,7 @@
         <v>11</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1325,11 +1322,11 @@
         <v>108</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G2" s="22">
         <f>MAX(A:A)</f>
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1354,7 +1351,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>108</v>
@@ -1393,13 +1390,13 @@
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
-        <v>27</v>
+        <v>251</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>108</v>
@@ -1410,16 +1407,16 @@
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
-        <v>89</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="F8" s="28" t="s">
         <v>18</v>
@@ -1427,13 +1424,13 @@
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>1</v>
@@ -1444,13 +1441,13 @@
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>1</v>
@@ -1461,13 +1458,13 @@
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>1</v>
@@ -1478,13 +1475,13 @@
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>1</v>
@@ -1495,44 +1492,44 @@
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
-        <v>67</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>18</v>
+        <v>87</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
@@ -1540,13 +1537,13 @@
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>9</v>
@@ -1554,13 +1551,13 @@
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
@@ -1568,41 +1565,41 @@
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>9</v>
@@ -1610,13 +1607,13 @@
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
@@ -1624,13 +1621,13 @@
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>9</v>
@@ -1638,13 +1635,13 @@
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>9</v>
@@ -1652,13 +1649,13 @@
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>9</v>
@@ -1666,13 +1663,13 @@
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>9</v>
@@ -1680,13 +1677,13 @@
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>9</v>
@@ -1694,13 +1691,13 @@
     </row>
     <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>9</v>
@@ -1708,13 +1705,13 @@
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>9</v>
@@ -1722,27 +1719,27 @@
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
-        <v>184</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>31</v>
+        <v>72</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>87</v>
@@ -1750,13 +1747,13 @@
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>171</v>
+        <v>92</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>87</v>
@@ -1764,27 +1761,27 @@
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>108</v>
@@ -1792,13 +1789,13 @@
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>108</v>
@@ -1806,13 +1803,13 @@
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>108</v>
@@ -1820,13 +1817,13 @@
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>108</v>
@@ -1834,7 +1831,7 @@
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>31</v>
@@ -1848,13 +1845,13 @@
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>108</v>
@@ -1862,13 +1859,13 @@
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>108</v>
@@ -1876,13 +1873,13 @@
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>108</v>
@@ -1890,27 +1887,27 @@
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
-        <v>146</v>
+        <v>191</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>87</v>
@@ -1918,13 +1915,13 @@
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>87</v>
@@ -1932,13 +1929,13 @@
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>87</v>
@@ -1946,27 +1943,27 @@
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
-        <v>115</v>
+        <v>185</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>153</v>
+        <v>95</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>108</v>
@@ -1974,13 +1971,13 @@
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20">
-        <v>203</v>
+        <v>119</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>108</v>
@@ -1988,27 +1985,27 @@
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>90</v>
+        <v>169</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>87</v>
@@ -2016,27 +2013,27 @@
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>108</v>
@@ -2044,13 +2041,13 @@
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>108</v>
@@ -2058,13 +2055,13 @@
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
-        <v>168</v>
+        <v>83</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>108</v>
@@ -2072,13 +2069,13 @@
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
-        <v>82</v>
+        <v>168</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>108</v>
@@ -2086,13 +2083,13 @@
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
-        <v>164</v>
+        <v>82</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>108</v>
@@ -2100,13 +2097,13 @@
     </row>
     <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>108</v>
@@ -2114,13 +2111,13 @@
     </row>
     <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>108</v>
@@ -2128,13 +2125,13 @@
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>108</v>
@@ -2142,13 +2139,13 @@
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
-        <v>165</v>
+        <v>81</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>108</v>
@@ -2156,13 +2153,13 @@
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20">
-        <v>80</v>
+        <v>165</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>108</v>
@@ -2170,41 +2167,41 @@
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
-        <v>202</v>
+        <v>80</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20">
-        <v>147</v>
+        <v>202</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>87</v>
@@ -2212,55 +2209,55 @@
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>159</v>
+        <v>85</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="20">
+        <v>113</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>87</v>
@@ -2268,13 +2265,13 @@
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="20">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>87</v>
@@ -2282,13 +2279,13 @@
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="20">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>87</v>
@@ -2296,13 +2293,13 @@
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>87</v>
@@ -2310,13 +2307,13 @@
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="20">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>87</v>
@@ -2324,13 +2321,13 @@
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="20">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>87</v>
@@ -2338,27 +2335,27 @@
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="20">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="21">
-        <v>149</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>100</v>
+      <c r="A74" s="20">
+        <v>148</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>87</v>
@@ -2366,21 +2363,21 @@
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="21">
-        <v>205</v>
+        <v>149</v>
       </c>
       <c r="B75" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>173</v>
+        <v>100</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B76" s="14" t="s">
         <v>31</v>
@@ -2393,28 +2390,28 @@
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="20">
-        <v>193</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>76</v>
+      <c r="A77" s="21">
+        <v>206</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="B78" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>1</v>
@@ -2422,41 +2419,41 @@
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
-        <v>9</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>13</v>
+        <v>85</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="B80" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="20">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="B81" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>108</v>
@@ -2464,13 +2461,13 @@
     </row>
     <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="20">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="B82" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>108</v>
@@ -2478,13 +2475,13 @@
     </row>
     <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="20">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B83" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>134</v>
+        <v>59</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>108</v>
@@ -2492,13 +2489,13 @@
     </row>
     <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B84" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>51</v>
+        <v>133</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>108</v>
@@ -2506,13 +2503,13 @@
     </row>
     <row r="85" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="B85" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>108</v>
@@ -2520,13 +2517,13 @@
     </row>
     <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="B86" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>108</v>
@@ -2534,13 +2531,13 @@
     </row>
     <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="20">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B87" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>108</v>
@@ -2548,13 +2545,13 @@
     </row>
     <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B88" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>108</v>
@@ -2562,13 +2559,13 @@
     </row>
     <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B89" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>108</v>
@@ -2576,13 +2573,13 @@
     </row>
     <row r="90" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="20">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B90" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>108</v>
@@ -2590,13 +2587,13 @@
     </row>
     <row r="91" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="20">
-        <v>199</v>
+        <v>18</v>
       </c>
       <c r="B91" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>108</v>
@@ -2604,41 +2601,41 @@
     </row>
     <row r="92" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="20">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="B92" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="20">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="B93" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="20">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B94" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>141</v>
+        <v>48</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>108</v>
@@ -2646,13 +2643,13 @@
     </row>
     <row r="95" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="20">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="B95" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>108</v>
@@ -2660,13 +2657,13 @@
     </row>
     <row r="96" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="20">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B96" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>108</v>
@@ -2674,41 +2671,41 @@
     </row>
     <row r="97" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="20">
-        <v>167</v>
+        <v>35</v>
       </c>
       <c r="B97" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>68</v>
+        <v>121</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="20">
-        <v>111</v>
+        <v>167</v>
       </c>
       <c r="B98" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="20">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="B99" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>108</v>
@@ -2716,13 +2713,13 @@
     </row>
     <row r="100" spans="1:4" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="20">
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="B100" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>108</v>
@@ -2730,13 +2727,13 @@
     </row>
     <row r="101" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="20">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B101" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>108</v>
@@ -2744,69 +2741,69 @@
     </row>
     <row r="102" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="20">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="B102" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="20">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="B103" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="20">
-        <v>187</v>
+        <v>103</v>
       </c>
       <c r="B104" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="20">
-        <v>132</v>
+        <v>187</v>
       </c>
       <c r="B105" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="20">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B106" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>167</v>
+        <v>17</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>108</v>
@@ -2814,13 +2811,13 @@
     </row>
     <row r="107" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="20">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B107" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>108</v>
@@ -2828,13 +2825,13 @@
     </row>
     <row r="108" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="20">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>108</v>
@@ -2842,13 +2839,13 @@
     </row>
     <row r="109" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="20">
-        <v>200</v>
+        <v>97</v>
       </c>
       <c r="B109" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>108</v>
@@ -2856,13 +2853,13 @@
     </row>
     <row r="110" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="20">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="B110" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>108</v>
@@ -2870,41 +2867,41 @@
     </row>
     <row r="111" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="20">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B111" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="20">
-        <v>201</v>
+        <v>26</v>
       </c>
       <c r="B112" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>150</v>
+        <v>72</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="20">
-        <v>106</v>
+        <v>201</v>
       </c>
       <c r="B113" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>108</v>
@@ -2912,55 +2909,55 @@
     </row>
     <row r="114" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="20">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="20">
-        <v>102</v>
+        <v>1</v>
       </c>
       <c r="B115" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="20">
-        <v>175</v>
+        <v>102</v>
       </c>
       <c r="B116" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="117" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="20">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>7</v>
@@ -2968,27 +2965,27 @@
     </row>
     <row r="118" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="20">
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="B118" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="20">
-        <v>140</v>
+        <v>34</v>
       </c>
       <c r="B119" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>108</v>
@@ -2996,27 +2993,27 @@
     </row>
     <row r="120" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="20">
-        <v>13</v>
+        <v>140</v>
       </c>
       <c r="B120" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="121" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="20">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B121" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>87</v>
@@ -3024,27 +3021,27 @@
     </row>
     <row r="122" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="20">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="B122" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="123" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="20">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="B123" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>108</v>
@@ -3052,13 +3049,13 @@
     </row>
     <row r="124" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="20">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="B124" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>108</v>
@@ -3066,13 +3063,13 @@
     </row>
     <row r="125" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="20">
-        <v>107</v>
+        <v>32</v>
       </c>
       <c r="B125" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>108</v>
@@ -3080,13 +3077,13 @@
     </row>
     <row r="126" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="20">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="B126" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>151</v>
+        <v>58</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>108</v>
@@ -3094,13 +3091,13 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="20">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B127" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>108</v>
@@ -3108,41 +3105,41 @@
     </row>
     <row r="128" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="20">
-        <v>23</v>
+        <v>142</v>
       </c>
       <c r="B128" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="129" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="20">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="B129" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="130" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="20">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B130" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>128</v>
+        <v>46</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>108</v>
@@ -3150,13 +3147,13 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="20">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="B131" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>108</v>
@@ -3164,13 +3161,13 @@
     </row>
     <row r="132" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="20">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B132" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>108</v>
@@ -3178,13 +3175,13 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="20">
-        <v>126</v>
+        <v>33</v>
       </c>
       <c r="B133" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>108</v>
@@ -3192,13 +3189,13 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="20">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B134" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>108</v>
@@ -3206,41 +3203,41 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="20">
-        <v>171</v>
+        <v>125</v>
       </c>
       <c r="B135" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="20">
-        <v>21</v>
+        <v>171</v>
       </c>
       <c r="B136" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="20">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B137" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>87</v>
@@ -3248,27 +3245,27 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="20">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="B138" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="20">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B139" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>108</v>
@@ -3276,13 +3273,13 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="20">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="B140" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>108</v>
@@ -3290,13 +3287,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="20">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B141" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>108</v>
@@ -3304,13 +3301,13 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="20">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="B142" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>108</v>
@@ -3318,13 +3315,13 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="20">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B143" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>133</v>
+        <v>38</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>108</v>
@@ -3332,13 +3329,13 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="20">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="B144" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>108</v>
@@ -3346,41 +3343,41 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="20">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="B145" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="20">
-        <v>135</v>
+        <v>2</v>
       </c>
       <c r="B146" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="20">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="B147" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>108</v>
@@ -3388,13 +3385,13 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="20">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="B148" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>108</v>
@@ -3402,83 +3399,83 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="20">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="B149" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="20">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B150" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="20">
-        <v>173</v>
+        <v>20</v>
       </c>
       <c r="B151" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="20">
-        <v>3</v>
+        <v>173</v>
       </c>
       <c r="B152" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="20">
-        <v>130</v>
+        <v>3</v>
       </c>
       <c r="B153" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>144</v>
+        <v>63</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="20">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B154" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>108</v>
@@ -3486,13 +3483,13 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="20">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="B155" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>143</v>
+        <v>50</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>108</v>
@@ -3500,13 +3497,13 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="20">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="B156" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>53</v>
+        <v>142</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>108</v>
@@ -3514,653 +3511,667 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="20">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="B157" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="20">
-        <v>136</v>
-      </c>
-      <c r="B158" s="16" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="B158" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>148</v>
+        <v>66</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="20">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B159" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="25">
-        <v>207</v>
-      </c>
-      <c r="B160" s="34" t="s">
-        <v>175</v>
+      <c r="A160" s="20">
+        <v>144</v>
+      </c>
+      <c r="B160" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>175</v>
+        <v>134</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="25">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B161" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C161" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="D161" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="25">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B162" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="25">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B163" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="25">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B164" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="25">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B165" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="25">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B166" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="25">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B167" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="25">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B168" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="25">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B169" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="25">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B170" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="25">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B171" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="25">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B172" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="25">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B173" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="25">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B174" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="25">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B175" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="25">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B176" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="25">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B177" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="25">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B178" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="25">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B179" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="25">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B180" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="25">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B181" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="25">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B182" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="25">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B183" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="25">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B184" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="C184" s="35" t="s">
-        <v>200</v>
+        <v>174</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="25">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B185" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>201</v>
+        <v>174</v>
+      </c>
+      <c r="C185" s="35" t="s">
+        <v>199</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="25">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B186" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="25">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B187" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="25">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B188" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="25">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B189" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="25">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B190" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="25">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B191" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="25">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B192" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C192" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="25">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B193" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="25">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B194" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="25">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B195" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="25">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B196" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="25">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B197" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="25">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B198" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C198" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="25">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B199" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C199" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="25">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B200" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="25">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B201" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="25">
+        <v>249</v>
+      </c>
+      <c r="B202" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="25">
         <v>250</v>
       </c>
-      <c r="B202" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="C202" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>175</v>
+      <c r="B203" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D159">
-    <sortCondition ref="B2:B159"/>
-    <sortCondition ref="C2:C159"/>
-    <sortCondition ref="A2:A159"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D160">
+    <sortCondition ref="B2:B160"/>
+    <sortCondition ref="C2:C160"/>
+    <sortCondition ref="A2:A160"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>